<commit_message>
change Add conc function
</commit_message>
<xml_diff>
--- a/01.04.19_MTT_Perkin_data/concentrations_2.xlsx
+++ b/01.04.19_MTT_Perkin_data/concentrations_2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Drug</t>
   </si>
@@ -127,13 +127,16 @@
   </si>
   <si>
     <t>DMSO</t>
+  </si>
+  <si>
+    <t>Dox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,23 +439,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +463,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -468,7 +471,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -476,7 +479,7 @@
         <v>10.94</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -484,7 +487,7 @@
         <v>8.0299999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -492,7 +495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -500,7 +503,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -508,7 +511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -516,7 +519,7 @@
         <v>8.24</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -524,7 +527,7 @@
         <v>10.54</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -532,7 +535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -540,7 +543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -548,7 +551,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -556,7 +559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -564,7 +567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -572,7 +575,7 @@
         <v>11.52</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -580,7 +583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -588,7 +591,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -596,7 +599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -604,7 +607,7 @@
         <v>12.69</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -612,7 +615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -620,7 +623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -628,7 +631,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -636,7 +639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -644,7 +647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -652,7 +655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -660,7 +663,7 @@
         <v>13.13</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -668,7 +671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -676,7 +679,7 @@
         <v>15.32</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -684,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -692,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -700,7 +703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -708,7 +711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -716,7 +719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -724,12 +727,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>